<commit_message>
corrected metadata readme, added other results folders and put in .gitignore
</commit_message>
<xml_diff>
--- a/PhyloseqObjects_forAnalysis/2019.04.26_SGvariety_Metadata_OutliersRmv_README.xlsx
+++ b/PhyloseqObjects_forAnalysis/2019.04.26_SGvariety_Metadata_OutliersRmv_README.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tayler Ulbrich\Documents\01_Grad School\02_Projects\01_SwitchgrassVariety\03_Data\Sequencing\Final_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tayler Ulbrich\Documents\01_Grad School\02_Projects\01_SwitchgrassVariety\Git_SGcultivar\PhyloseqObjects_forAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5E7399-2198-4814-9DDB-DFAA8A9FDDFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D0901D-B918-41F5-8FBE-ECE7099FAE28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="10005" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2019.02.13_SGvariety_Metadata_O" sheetId="2" r:id="rId1"/>
+    <sheet name="Read Me" sheetId="2" r:id="rId1"/>
     <sheet name="2019.04.26_SGvariety_Metadata_O" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2224" uniqueCount="593">
   <si>
     <t>X.SampleID</t>
   </si>
@@ -1602,9 +1602,6 @@
     <t>DryRoot_g/(WetRoot_EnvWt_G-EnvWt_g)</t>
   </si>
   <si>
-    <t>DryWetRoot_ratio * WetRootWeight_total_g</t>
-  </si>
-  <si>
     <t>DryRootWt_total_g/Network_length</t>
   </si>
   <si>
@@ -1617,78 +1614,12 @@
     <t>Network_length/98.17 (aka the volume of soil collected: 20cm length * 1.25cm radius core = volume 98.17cm3)</t>
   </si>
   <si>
-    <t xml:space="preserve">percent water in the soil </t>
-  </si>
-  <si>
-    <t>percent N in the soil, measured by combustion on elemental analyzer</t>
-  </si>
-  <si>
-    <t>percent of N in soil from fixation</t>
-  </si>
-  <si>
-    <t>fixation rate in soil, units of g N/vial/d</t>
-  </si>
-  <si>
-    <t>fixation rate in soil, units of ug N/g soil/d</t>
-  </si>
-  <si>
-    <t>nitrate concentration in soil on the first day of the mineralization incubations, in ug N/g soil</t>
-  </si>
-  <si>
-    <t>ammonium concentration in soil on the first day of the mineralization incubations, in ug N/g soil</t>
-  </si>
-  <si>
-    <t>nitrate concentration in soil on the seventh day of the mineralization incubations, in ug N/g soil</t>
-  </si>
-  <si>
-    <t>ammonium concentration in soil on the seventh day of the mineralization incubations, in ug N/g soil</t>
-  </si>
-  <si>
-    <t>length of incubation in days</t>
-  </si>
-  <si>
-    <t>mineralization rate, in ug N/g soil/d</t>
-  </si>
-  <si>
-    <t>nitrification rate, in ug N/g soil/d</t>
-  </si>
-  <si>
-    <t>percent water in the roots</t>
-  </si>
-  <si>
-    <t>percent N in the roots, measured by combustion on elemental analyzer</t>
-  </si>
-  <si>
-    <t>percent of N in roots from fixation</t>
-  </si>
-  <si>
-    <t>root fixation rate, in g N/vial/d</t>
-  </si>
-  <si>
-    <t>root fixation rate, in ug N/g root/d</t>
-  </si>
-  <si>
-    <t>year harvested</t>
-  </si>
-  <si>
     <t>date of harvest</t>
   </si>
   <si>
     <t>year variety was planted</t>
   </si>
   <si>
-    <t>percent water in switchgrass at harvest</t>
-  </si>
-  <si>
-    <t>switchgrass yield in tons per acre</t>
-  </si>
-  <si>
-    <t>switchgrass yield in Mg/ha</t>
-  </si>
-  <si>
-    <t>total inorganic N (NO3 + NH4) in soil, in ug N/g soil, on the first day of mineralization incubations</t>
-  </si>
-  <si>
     <t>percent_soil_moisture_dry_weight_GravWaterContent or the wetsoil weight - dry soil weight/dry soil weight</t>
   </si>
   <si>
@@ -1795,13 +1726,110 @@
   </si>
   <si>
     <t>Ammonium ugN per g dry soil (NO3 colormetric assay with K2SO4)  - removed two outliers (C8 and B10) that were removed from SMC data for being outliers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes for TCU's data collection </t>
+  </si>
+  <si>
+    <t>DryWetRoot_ratio * WetRootWeight_total_g (this value is used for analysis and calculation of SRL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tayler Ulbrich </t>
+  </si>
+  <si>
+    <t>Metadata read me file</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">measurements indicated with SR were collected by Sarah Roley and detailed in Roley et al. (2020) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Phytobiomes</t>
+    </r>
+  </si>
+  <si>
+    <t>percent water in the soil - SR</t>
+  </si>
+  <si>
+    <t>percent N in the soil, measured by combustion on elemental analyzer - SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percent of N in soil from fixation -SR </t>
+  </si>
+  <si>
+    <t>fixation rate in soil, units of g N/vial/d - SR</t>
+  </si>
+  <si>
+    <t>fixation rate in soil, units of ug N/g soil/d - SR</t>
+  </si>
+  <si>
+    <t>nitrate concentration in soil on the first day of the mineralization incubations, in ug N/g soil- SR</t>
+  </si>
+  <si>
+    <t>ammonium concentration in soil on the first day of the mineralization incubations, in ug N/g soil- SR</t>
+  </si>
+  <si>
+    <t>nitrate concentration in soil on the seventh day of the mineralization incubations, in ug N/g soil- SR</t>
+  </si>
+  <si>
+    <t>ammonium concentration in soil on the seventh day of the mineralization incubations, in ug N/g soil- SR</t>
+  </si>
+  <si>
+    <t>length of incubation in days- SR</t>
+  </si>
+  <si>
+    <t>mineralization rate, in ug N/g soil/d- SR</t>
+  </si>
+  <si>
+    <t>nitrification rate, in ug N/g soil/d- SR</t>
+  </si>
+  <si>
+    <t>percent water in the roots- SR</t>
+  </si>
+  <si>
+    <t>percent N in the roots, measured by combustion on elemental analyzer- SR</t>
+  </si>
+  <si>
+    <t>percent of N in roots from fixation- SR</t>
+  </si>
+  <si>
+    <t>root fixation rate, in g N/vial/d- SR</t>
+  </si>
+  <si>
+    <t>root fixation rate, in ug N/g root/d- SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes from Sarah Roley's N measurements (identified by SR) </t>
+  </si>
+  <si>
+    <t>year harvest</t>
+  </si>
+  <si>
+    <t>percent water in switchgrass at harvest -SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switchgrass yield in tons per acre -SR </t>
+  </si>
+  <si>
+    <t>switchgrass yield in Mg/ha -SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total inorganic N (NO3 + NH4) in soil, in ug N/g soil, on the first day of mineralization incubations -SR </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1932,6 +1960,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2278,12 +2314,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2639,10 +2676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25:G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2652,659 +2689,633 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>502</v>
+        <v>567</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>503</v>
+      <c r="A2" s="5" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>505</v>
+        <v>569</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>577</v>
+        <v>513</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>578</v>
+        <v>514</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>579</v>
+        <v>515</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>583</v>
+        <v>516</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>580</v>
+        <v>554</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>581</v>
+        <v>555</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>582</v>
+        <v>556</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>517</v>
+        <v>560</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>518</v>
+        <v>557</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>519</v>
+        <v>558</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>520</v>
+        <v>559</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>524</v>
+        <v>565</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A36" t="s">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B36" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>527</v>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A39" t="s">
+        <v>548</v>
+      </c>
+      <c r="B39" t="s">
+        <v>549</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A35" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A43" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A44" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A47" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A50" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A52" t="s">
+        <v>550</v>
+      </c>
+      <c r="B52" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A53" t="s">
+        <v>551</v>
+      </c>
+      <c r="B53" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A54" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B54" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A55" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="B55" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A57" t="s">
+        <v>33</v>
+      </c>
+      <c r="B57" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B58" t="s">
         <v>571</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A59" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" t="s">
-        <v>528</v>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A60" t="s">
+        <v>36</v>
+      </c>
+      <c r="B60" t="s">
+        <v>573</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" t="s">
-        <v>529</v>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A61" t="s">
+        <v>37</v>
+      </c>
+      <c r="B61" t="s">
+        <v>574</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A38" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" t="s">
-        <v>530</v>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" t="s">
+        <v>575</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A39" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" t="s">
-        <v>531</v>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A63" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" t="s">
+        <v>576</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A41" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A42" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A43" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A64" t="s">
         <v>40</v>
       </c>
-      <c r="B43" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A44" t="s">
-        <v>41</v>
-      </c>
-      <c r="B44" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A45" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A48" t="s">
-        <v>45</v>
-      </c>
-      <c r="B48" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A49" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" t="s">
-        <v>46</v>
-      </c>
-      <c r="C49" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A50" t="s">
-        <v>47</v>
-      </c>
-      <c r="B50" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B51" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A52" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" t="s">
-        <v>49</v>
-      </c>
-      <c r="C52" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A53" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A54" t="s">
-        <v>51</v>
-      </c>
-      <c r="B54" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A55" t="s">
-        <v>52</v>
-      </c>
-      <c r="B55" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A56" t="s">
-        <v>53</v>
-      </c>
-      <c r="B56" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A57" t="s">
-        <v>54</v>
-      </c>
-      <c r="B57" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A58" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A59" t="s">
-        <v>56</v>
-      </c>
-      <c r="B59" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A60" t="s">
-        <v>57</v>
-      </c>
-      <c r="B60" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A61" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A62" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A63" t="s">
-        <v>61</v>
-      </c>
-      <c r="B63" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A64" t="s">
-        <v>62</v>
-      </c>
       <c r="B64" t="s">
-        <v>555</v>
+        <v>577</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="B65" t="s">
-        <v>556</v>
+        <v>578</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>557</v>
+        <v>592</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B67" t="s">
-        <v>558</v>
+        <v>579</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B68" t="s">
-        <v>559</v>
+        <v>580</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="B69" t="s">
-        <v>560</v>
+        <v>581</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B70" t="s">
-        <v>561</v>
+        <v>582</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B71" t="s">
-        <v>563</v>
+        <v>583</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B72" t="s">
-        <v>562</v>
+        <v>584</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A73" t="s">
-        <v>573</v>
+        <v>48</v>
       </c>
       <c r="B73" t="s">
-        <v>575</v>
+        <v>585</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A74" t="s">
-        <v>574</v>
+        <v>49</v>
       </c>
       <c r="B74" t="s">
-        <v>576</v>
+        <v>586</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A75" s="4" t="s">
-        <v>584</v>
+      <c r="A75" t="s">
+        <v>51</v>
       </c>
       <c r="B75" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A76" s="4" t="s">
-        <v>585</v>
+      <c r="A76" t="s">
+        <v>52</v>
       </c>
       <c r="B76" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A77" t="s">
+        <v>53</v>
+      </c>
+      <c r="B77" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A78" t="s">
+        <v>54</v>
+      </c>
+      <c r="B78" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A79" t="s">
+        <v>55</v>
+      </c>
+      <c r="B79" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A80" t="s">
+        <v>56</v>
+      </c>
+      <c r="B80" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A81" t="s">
+        <v>50</v>
+      </c>
+      <c r="B81" t="s">
         <v>587</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3437,7 +3448,7 @@
         <v>32</v>
       </c>
       <c r="AK1" t="s">
-        <v>571</v>
+        <v>548</v>
       </c>
       <c r="AL1" t="s">
         <v>33</v>
@@ -3545,25 +3556,25 @@
         <v>68</v>
       </c>
       <c r="BV1" s="4" t="s">
-        <v>573</v>
+        <v>550</v>
       </c>
       <c r="BW1" s="4" t="s">
-        <v>574</v>
+        <v>551</v>
       </c>
       <c r="BX1" s="4" t="s">
-        <v>584</v>
+        <v>561</v>
       </c>
       <c r="BY1" s="4" t="s">
-        <v>585</v>
+        <v>562</v>
       </c>
       <c r="BZ1" t="s">
-        <v>564</v>
+        <v>541</v>
       </c>
       <c r="CA1" t="s">
-        <v>570</v>
+        <v>547</v>
       </c>
       <c r="CB1" t="s">
-        <v>565</v>
+        <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:80" x14ac:dyDescent="0.75">
@@ -10006,7 +10017,7 @@
         <v>42640</v>
       </c>
       <c r="CB29" t="s">
-        <v>567</v>
+        <v>544</v>
       </c>
     </row>
     <row r="30" spans="1:80" x14ac:dyDescent="0.75">
@@ -16219,7 +16230,7 @@
         <v>42636</v>
       </c>
       <c r="CB56" t="s">
-        <v>566</v>
+        <v>543</v>
       </c>
     </row>
     <row r="57" spans="1:80" x14ac:dyDescent="0.75">
@@ -27068,7 +27079,7 @@
         <v>42641</v>
       </c>
       <c r="CB103" t="s">
-        <v>568</v>
+        <v>545</v>
       </c>
     </row>
     <row r="104" spans="1:80" x14ac:dyDescent="0.75">
@@ -39291,7 +39302,7 @@
         <v>42641</v>
       </c>
       <c r="CB156" t="s">
-        <v>569</v>
+        <v>546</v>
       </c>
     </row>
     <row r="157" spans="1:80" x14ac:dyDescent="0.75">

</xml_diff>